<commit_message>
updated with latest changes in mapping
</commit_message>
<xml_diff>
--- a/dev/energyscope_data/CA-QC/unit_conversion_3.10.xlsx
+++ b/dev/energyscope_data/CA-QC/unit_conversion_3.10.xlsx
@@ -2936,7 +2936,7 @@
         <v>621</v>
       </c>
       <c r="C12">
-        <f>(8760*0.85)/130 / 1000000</f>
+        <f> (8760*0.85)/130 / 1000000</f>
         <v>0</v>
       </c>
       <c r="D12" t="s">
@@ -2977,7 +2977,7 @@
         <v>621</v>
       </c>
       <c r="C14">
-        <f>(8760*0.85)/130 / 1000000</f>
+        <f> (8760*0.85)/130 / 1000000</f>
         <v>0</v>
       </c>
       <c r="D14" t="s">
@@ -3039,7 +3039,7 @@
         <v>622</v>
       </c>
       <c r="C17">
-        <f>1 / (13.9 * 0.716)</f>
+        <f> 1 / (13.9 * 0.716)</f>
         <v>0</v>
       </c>
       <c r="D17" t="s">
@@ -3080,7 +3080,7 @@
         <v>622</v>
       </c>
       <c r="C19">
-        <f>1 / (0.716 * 13.9 * 0.4)</f>
+        <f> 1 / (0.716 * 13.9 * 0.4)</f>
         <v>0</v>
       </c>
       <c r="D19" t="s">
@@ -3101,7 +3101,7 @@
         <v>621</v>
       </c>
       <c r="C20">
-        <f>1000000 / 160</f>
+        <f> 1000000 / 160</f>
         <v>0</v>
       </c>
       <c r="D20" t="s">
@@ -3119,7 +3119,7 @@
         <v>621</v>
       </c>
       <c r="C21">
-        <f>3.6 * 8760 * 0.86 * 7.72 / (10 * 8.279)</f>
+        <f> 3.6 * 8760 * 0.86 * 7.72 / (10 * 8.279)</f>
         <v>0</v>
       </c>
       <c r="D21" t="s">
@@ -3241,7 +3241,8 @@
         <v>621</v>
       </c>
       <c r="C27">
-        <f>0.00000000254628/5.34876232801608E-10</f>
+        <f>0.00000000254628/0.000000000534876232801608
+</f>
         <v>0</v>
       </c>
       <c r="D27" t="s">
@@ -3279,7 +3280,8 @@
         <v>621</v>
       </c>
       <c r="C29">
-        <f>0.00000000254628/5.34874716181652E-10</f>
+        <f>0.00000000254628/0.000000000534874716181652
+</f>
         <v>0</v>
       </c>
       <c r="D29" t="s">
@@ -3443,7 +3445,8 @@
         <v>621</v>
       </c>
       <c r="C37">
-        <f>0.00000000254628/5.34874716181652E-10</f>
+        <f>0.00000000254628/0.000000000534874716181652
+</f>
         <v>0</v>
       </c>
       <c r="D37" t="s">
@@ -3481,7 +3484,8 @@
         <v>621</v>
       </c>
       <c r="C39">
-        <f>0.00000000254628/5.34874716181652E-10</f>
+        <f>0.00000000254628/0.000000000534874716181652
+</f>
         <v>0</v>
       </c>
       <c r="D39" t="s">
@@ -3645,7 +3649,8 @@
         <v>621</v>
       </c>
       <c r="C47">
-        <f>0.00000000254628/5.3483199147628E-10</f>
+        <f>0.00000000254628/0.00000000053483199147628
+</f>
         <v>0</v>
       </c>
       <c r="D47" t="s">
@@ -3683,7 +3688,8 @@
         <v>621</v>
       </c>
       <c r="C49">
-        <f>0.00000000254628/5.3483199147628E-10</f>
+        <f>0.00000000254628/0.00000000053483199147628
+</f>
         <v>0</v>
       </c>
       <c r="D49" t="s">
@@ -3793,7 +3799,8 @@
         <v>621</v>
       </c>
       <c r="C55">
-        <f>0.00000000254628/5.3483199147628E-10</f>
+        <f>0.00000000254628/0.00000000053483199147628
+</f>
         <v>0</v>
       </c>
       <c r="D55" t="s">
@@ -3831,7 +3838,8 @@
         <v>621</v>
       </c>
       <c r="C57">
-        <f>0.00000000254628/5.3483199147628E-10</f>
+        <f>0.00000000254628/0.00000000053483199147628
+</f>
         <v>0</v>
       </c>
       <c r="D57" t="s">
@@ -3941,7 +3949,8 @@
         <v>621</v>
       </c>
       <c r="C63">
-        <f>0.00000000254628/5.3483199147628E-10</f>
+        <f>0.00000000254628/0.00000000053483199147628
+</f>
         <v>0</v>
       </c>
       <c r="D63" t="s">
@@ -3979,7 +3988,8 @@
         <v>621</v>
       </c>
       <c r="C65">
-        <f>0.00000000254628/5.3483199147628E-10</f>
+        <f>0.00000000254628/0.00000000053483199147628
+</f>
         <v>0</v>
       </c>
       <c r="D65" t="s">
@@ -4021,7 +4031,7 @@
         <v>621</v>
       </c>
       <c r="C67">
-        <f>1 * 8760 * 0.297 / (13 * 50000)</f>
+        <f> 1 * 8760 * 0.297 / (13 * 50000)</f>
         <v>0</v>
       </c>
       <c r="D67" t="s">
@@ -4063,7 +4073,7 @@
         <v>621</v>
       </c>
       <c r="C69">
-        <f>1 * 8760 * 0.297 / (13 * 50000)</f>
+        <f> 1 * 8760 * 0.297 / (13 * 50000)</f>
         <v>0</v>
       </c>
       <c r="D69" t="s">
@@ -4105,7 +4115,7 @@
         <v>621</v>
       </c>
       <c r="C71">
-        <f>1 * 8760 * 0.297 / (13 * 50000)</f>
+        <f> 1 * 8760 * 0.297 / (13 * 50000)</f>
         <v>0</v>
       </c>
       <c r="D71" t="s">
@@ -4147,7 +4157,7 @@
         <v>621</v>
       </c>
       <c r="C73">
-        <f>1 * 8760 * 0.297 / (13 * 50000)</f>
+        <f> 1 * 8760 * 0.297 / (13 * 50000)</f>
         <v>0</v>
       </c>
       <c r="D73" t="s">
@@ -4189,7 +4199,7 @@
         <v>621</v>
       </c>
       <c r="C75">
-        <f>1 * 8760 * 0.297 / (13 * 50000)</f>
+        <f> 1 * 8760 * 0.297 / (13 * 50000)</f>
         <v>0</v>
       </c>
       <c r="D75" t="s">
@@ -4231,7 +4241,7 @@
         <v>621</v>
       </c>
       <c r="C77">
-        <f>1 * 8760 * 0.297 / (13 * 50000)</f>
+        <f> 1 * 8760 * 0.297 / (13 * 50000)</f>
         <v>0</v>
       </c>
       <c r="D77" t="s">
@@ -4273,7 +4283,7 @@
         <v>621</v>
       </c>
       <c r="C79">
-        <f>1 * 8760 * 0.297 / (13 * 50000)</f>
+        <f> 1 * 8760 * 0.297 / (13 * 50000)</f>
         <v>0</v>
       </c>
       <c r="D79" t="s">
@@ -4315,7 +4325,7 @@
         <v>621</v>
       </c>
       <c r="C81">
-        <f>1 * 8760 * 0.297 / (13 * 50000)</f>
+        <f> 1 * 8760 * 0.297 / (13 * 50000)</f>
         <v>0</v>
       </c>
       <c r="D81" t="s">
@@ -4357,7 +4367,7 @@
         <v>621</v>
       </c>
       <c r="C83">
-        <f>1 * 8760 * 0.297 / (13 * 50000)</f>
+        <f> 1 * 8760 * 0.297 / (13 * 50000)</f>
         <v>0</v>
       </c>
       <c r="D83" t="s">
@@ -4399,7 +4409,7 @@
         <v>621</v>
       </c>
       <c r="C85">
-        <f>1 * 8760 * 0.297 / (13 * 50000)</f>
+        <f> 1 * 8760 * 0.297 / (13 * 50000)</f>
         <v>0</v>
       </c>
       <c r="D85" t="s">
@@ -4441,7 +4451,7 @@
         <v>621</v>
       </c>
       <c r="C87">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D87" t="s">
@@ -4483,7 +4493,7 @@
         <v>621</v>
       </c>
       <c r="C89">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D89" t="s">
@@ -4525,7 +4535,7 @@
         <v>621</v>
       </c>
       <c r="C91">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D91" t="s">
@@ -4567,7 +4577,7 @@
         <v>621</v>
       </c>
       <c r="C93">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D93" t="s">
@@ -4609,7 +4619,7 @@
         <v>621</v>
       </c>
       <c r="C95">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D95" t="s">
@@ -4651,7 +4661,7 @@
         <v>621</v>
       </c>
       <c r="C97">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D97" t="s">
@@ -4693,7 +4703,7 @@
         <v>621</v>
       </c>
       <c r="C99">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D99" t="s">
@@ -4735,7 +4745,7 @@
         <v>621</v>
       </c>
       <c r="C101">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D101" t="s">
@@ -4777,7 +4787,7 @@
         <v>621</v>
       </c>
       <c r="C103">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D103" t="s">
@@ -4819,7 +4829,7 @@
         <v>621</v>
       </c>
       <c r="C105">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D105" t="s">
@@ -4861,7 +4871,7 @@
         <v>621</v>
       </c>
       <c r="C107">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D107" t="s">
@@ -4903,7 +4913,7 @@
         <v>621</v>
       </c>
       <c r="C109">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D109" t="s">
@@ -4945,7 +4955,7 @@
         <v>621</v>
       </c>
       <c r="C111">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D111" t="s">
@@ -4987,7 +4997,7 @@
         <v>621</v>
       </c>
       <c r="C113">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D113" t="s">
@@ -5029,7 +5039,7 @@
         <v>621</v>
       </c>
       <c r="C115">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D115" t="s">
@@ -5071,7 +5081,7 @@
         <v>621</v>
       </c>
       <c r="C117">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D117" t="s">
@@ -5113,7 +5123,7 @@
         <v>621</v>
       </c>
       <c r="C119">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D119" t="s">
@@ -5155,7 +5165,7 @@
         <v>621</v>
       </c>
       <c r="C121">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D121" t="s">
@@ -5197,7 +5207,7 @@
         <v>621</v>
       </c>
       <c r="C123">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D123" t="s">
@@ -5239,7 +5249,7 @@
         <v>621</v>
       </c>
       <c r="C125">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D125" t="s">
@@ -5281,7 +5291,7 @@
         <v>621</v>
       </c>
       <c r="C127">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D127" t="s">
@@ -5323,7 +5333,7 @@
         <v>621</v>
       </c>
       <c r="C129">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D129" t="s">
@@ -5365,7 +5375,7 @@
         <v>621</v>
       </c>
       <c r="C131">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D131" t="s">
@@ -5407,7 +5417,7 @@
         <v>621</v>
       </c>
       <c r="C133">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D133" t="s">
@@ -5449,7 +5459,7 @@
         <v>621</v>
       </c>
       <c r="C135">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D135" t="s">
@@ -5491,7 +5501,7 @@
         <v>621</v>
       </c>
       <c r="C137">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D137" t="s">
@@ -5533,7 +5543,7 @@
         <v>621</v>
       </c>
       <c r="C139">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D139" t="s">
@@ -5575,7 +5585,7 @@
         <v>621</v>
       </c>
       <c r="C141">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D141" t="s">
@@ -5617,7 +5627,7 @@
         <v>621</v>
       </c>
       <c r="C143">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D143" t="s">
@@ -5659,7 +5669,7 @@
         <v>621</v>
       </c>
       <c r="C145">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D145" t="s">
@@ -5701,7 +5711,7 @@
         <v>621</v>
       </c>
       <c r="C147">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D147" t="s">
@@ -5743,7 +5753,7 @@
         <v>621</v>
       </c>
       <c r="C149">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D149" t="s">
@@ -5785,7 +5795,7 @@
         <v>621</v>
       </c>
       <c r="C151">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D151" t="s">
@@ -5827,7 +5837,7 @@
         <v>621</v>
       </c>
       <c r="C153">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D153" t="s">
@@ -5869,7 +5879,7 @@
         <v>621</v>
       </c>
       <c r="C155">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D155" t="s">
@@ -5911,7 +5921,7 @@
         <v>621</v>
       </c>
       <c r="C157">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D157" t="s">
@@ -5953,7 +5963,7 @@
         <v>621</v>
       </c>
       <c r="C159">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D159" t="s">
@@ -5995,7 +6005,7 @@
         <v>621</v>
       </c>
       <c r="C161">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D161" t="s">
@@ -6037,7 +6047,7 @@
         <v>621</v>
       </c>
       <c r="C163">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D163" t="s">
@@ -6079,7 +6089,7 @@
         <v>621</v>
       </c>
       <c r="C165">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D165" t="s">
@@ -6121,7 +6131,7 @@
         <v>621</v>
       </c>
       <c r="C167">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D167" t="s">
@@ -6163,7 +6173,7 @@
         <v>621</v>
       </c>
       <c r="C169">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D169" t="s">
@@ -6205,7 +6215,7 @@
         <v>621</v>
       </c>
       <c r="C171">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D171" t="s">
@@ -6247,7 +6257,7 @@
         <v>621</v>
       </c>
       <c r="C173">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D173" t="s">
@@ -6289,7 +6299,7 @@
         <v>621</v>
       </c>
       <c r="C175">
-        <f>1 * 8760 * 0.051 / (1.5 * 7600)</f>
+        <f> 1 * 8760 * 0.051 / (1.5 * 7600)</f>
         <v>0</v>
       </c>
       <c r="D175" t="s">
@@ -6331,7 +6341,7 @@
         <v>621</v>
       </c>
       <c r="C177">
-        <f>1 * 8760 * 0.051 / (1.5 * 7600)</f>
+        <f> 1 * 8760 * 0.051 / (1.5 * 7600)</f>
         <v>0</v>
       </c>
       <c r="D177" t="s">
@@ -6373,7 +6383,7 @@
         <v>621</v>
       </c>
       <c r="C179">
-        <f>1 * 8760 * 0.051 / (1.5 * 7600)</f>
+        <f> 1 * 8760 * 0.051 / (1.5 * 7600)</f>
         <v>0</v>
       </c>
       <c r="D179" t="s">
@@ -6415,7 +6425,7 @@
         <v>621</v>
       </c>
       <c r="C181">
-        <f>1 * 8760 * 0.051 / (1.5 * 7600)</f>
+        <f> 1 * 8760 * 0.051 / (1.5 * 7600)</f>
         <v>0</v>
       </c>
       <c r="D181" t="s">
@@ -6457,7 +6467,7 @@
         <v>621</v>
       </c>
       <c r="C183">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D183" t="s">
@@ -6499,7 +6509,7 @@
         <v>621</v>
       </c>
       <c r="C185">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D185" t="s">
@@ -6541,7 +6551,7 @@
         <v>621</v>
       </c>
       <c r="C187">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D187" t="s">
@@ -6583,7 +6593,7 @@
         <v>621</v>
       </c>
       <c r="C189">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D189" t="s">
@@ -6625,7 +6635,7 @@
         <v>621</v>
       </c>
       <c r="C191">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D191" t="s">
@@ -6667,7 +6677,7 @@
         <v>621</v>
       </c>
       <c r="C193">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D193" t="s">
@@ -6709,7 +6719,7 @@
         <v>621</v>
       </c>
       <c r="C195">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D195" t="s">
@@ -6751,7 +6761,7 @@
         <v>621</v>
       </c>
       <c r="C197">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D197" t="s">
@@ -6988,7 +6998,7 @@
         <v>621</v>
       </c>
       <c r="C209">
-        <f>1 / (16000*827.3)</f>
+        <f> 1 / (16000*827.3)</f>
         <v>0</v>
       </c>
       <c r="D209" t="s">
@@ -7009,7 +7019,7 @@
         <v>621</v>
       </c>
       <c r="C210">
-        <f>(1 / 1.5385) * (8760 * 0.86) / (33.3 * 1000) / 1000000</f>
+        <f> (1 / 1.5385) * (8760 * 0.86) / (33.3 * 1000) / 1000000</f>
         <v>0</v>
       </c>
       <c r="D210" t="s">
@@ -7051,7 +7061,7 @@
         <v>621</v>
       </c>
       <c r="C212">
-        <f>(1 / 1.190476) * (8760 * 0.86) / (33.3 * 1000) / 1000000</f>
+        <f> (1 / 1.190476) * (8760 * 0.86) / (33.3 * 1000) / 1000000</f>
         <v>0</v>
       </c>
       <c r="D212" t="s">
@@ -7072,7 +7082,7 @@
         <v>622</v>
       </c>
       <c r="C213">
-        <f>1 * 3.6 / 43</f>
+        <f> 1 * 3.6 / 43</f>
         <v>0</v>
       </c>
       <c r="D213" t="s">
@@ -7093,7 +7103,7 @@
         <v>621</v>
       </c>
       <c r="C214">
-        <f>1 * 8760 * 0.297 / (21 * 50000)</f>
+        <f> 1 * 8760 * 0.297 / (21 * 50000)</f>
         <v>0</v>
       </c>
       <c r="D214" t="s">
@@ -7135,7 +7145,7 @@
         <v>621</v>
       </c>
       <c r="C216">
-        <f>1 * 8760 * 0.297 / (21 * 50000)</f>
+        <f> 1 * 8760 * 0.297 / (21 * 50000)</f>
         <v>0</v>
       </c>
       <c r="D216" t="s">
@@ -7177,7 +7187,7 @@
         <v>621</v>
       </c>
       <c r="C218">
-        <f>1 * 8760 * 0.297 / (21 * 50000)</f>
+        <f> 1 * 8760 * 0.297 / (21 * 50000)</f>
         <v>0</v>
       </c>
       <c r="D218" t="s">
@@ -7219,7 +7229,7 @@
         <v>621</v>
       </c>
       <c r="C220">
-        <f>1 * 8760 * 0.297 / (21 * 50000)</f>
+        <f> 1 * 8760 * 0.297 / (21 * 50000)</f>
         <v>0</v>
       </c>
       <c r="D220" t="s">
@@ -7261,7 +7271,7 @@
         <v>621</v>
       </c>
       <c r="C222">
-        <f>1 * 8760 * 0.297 / (21 * 50000)</f>
+        <f> 1 * 8760 * 0.297 / (21 * 50000)</f>
         <v>0</v>
       </c>
       <c r="D222" t="s">
@@ -7303,7 +7313,7 @@
         <v>621</v>
       </c>
       <c r="C224">
-        <f>1 * 8760 * 0.297 / (21 * 50000)</f>
+        <f> 1 * 8760 * 0.297 / (21 * 50000)</f>
         <v>0</v>
       </c>
       <c r="D224" t="s">
@@ -7345,7 +7355,7 @@
         <v>621</v>
       </c>
       <c r="C226">
-        <f>1 * 8760 * 0.297 / (21 * 50000)</f>
+        <f> 1 * 8760 * 0.297 / (21 * 50000)</f>
         <v>0</v>
       </c>
       <c r="D226" t="s">
@@ -7387,7 +7397,7 @@
         <v>621</v>
       </c>
       <c r="C228">
-        <f>1 * 8760 * 0.297 / (21 * 50000)</f>
+        <f> 1 * 8760 * 0.297 / (21 * 50000)</f>
         <v>0</v>
       </c>
       <c r="D228" t="s">
@@ -7429,7 +7439,7 @@
         <v>621</v>
       </c>
       <c r="C230">
-        <f>1 * 8760 * 0.297 / (21 * 50000)</f>
+        <f> 1 * 8760 * 0.297 / (21 * 50000)</f>
         <v>0</v>
       </c>
       <c r="D230" t="s">
@@ -7471,7 +7481,7 @@
         <v>621</v>
       </c>
       <c r="C232">
-        <f>1 * 8760 * 0.297 / (21 * 50000)</f>
+        <f> 1 * 8760 * 0.297 / (21 * 50000)</f>
         <v>0</v>
       </c>
       <c r="D232" t="s">
@@ -7513,7 +7523,7 @@
         <v>621</v>
       </c>
       <c r="C234">
-        <f>1 * 8760 * 0.297 / (21 * 50000)</f>
+        <f> 1 * 8760 * 0.297 / (21 * 50000)</f>
         <v>0</v>
       </c>
       <c r="D234" t="s">
@@ -7555,7 +7565,7 @@
         <v>621</v>
       </c>
       <c r="C236">
-        <f>1 * 8760 * 0.297 / (21 * 50000)</f>
+        <f> 1 * 8760 * 0.297 / (21 * 50000)</f>
         <v>0</v>
       </c>
       <c r="D236" t="s">
@@ -7597,7 +7607,7 @@
         <v>621</v>
       </c>
       <c r="C238">
-        <f>1 * 8760 * 0.297 / (21 * 50000)</f>
+        <f> 1 * 8760 * 0.297 / (21 * 50000)</f>
         <v>0</v>
       </c>
       <c r="D238" t="s">
@@ -7639,7 +7649,7 @@
         <v>621</v>
       </c>
       <c r="C240">
-        <f>1 * 8760 * 0.297 / (21 * 50000)</f>
+        <f> 1 * 8760 * 0.297 / (21 * 50000)</f>
         <v>0</v>
       </c>
       <c r="D240" t="s">
@@ -7681,7 +7691,7 @@
         <v>621</v>
       </c>
       <c r="C242">
-        <f>1 * 8760 * 0.297 / (21 * 50000)</f>
+        <f> 1 * 8760 * 0.297 / (21 * 50000)</f>
         <v>0</v>
       </c>
       <c r="D242" t="s">
@@ -7723,7 +7733,7 @@
         <v>621</v>
       </c>
       <c r="C244">
-        <f>1 * 8760 * 0.297 / (21 * 50000)</f>
+        <f> 1 * 8760 * 0.297 / (21 * 50000)</f>
         <v>0</v>
       </c>
       <c r="D244" t="s">
@@ -7765,7 +7775,7 @@
         <v>621</v>
       </c>
       <c r="C246">
-        <f>1 * 8760 * 0.297 / (21 * 50000)</f>
+        <f> 1 * 8760 * 0.297 / (21 * 50000)</f>
         <v>0</v>
       </c>
       <c r="D246" t="s">
@@ -7807,7 +7817,7 @@
         <v>621</v>
       </c>
       <c r="C248">
-        <f>1 * 8760 * 0.297 / (21 * 50000)</f>
+        <f> 1 * 8760 * 0.297 / (21 * 50000)</f>
         <v>0</v>
       </c>
       <c r="D248" t="s">
@@ -7849,7 +7859,7 @@
         <v>621</v>
       </c>
       <c r="C250">
-        <f>1 * 8760 * 0.297 / (21 * 50000)</f>
+        <f> 1 * 8760 * 0.297 / (21 * 50000)</f>
         <v>0</v>
       </c>
       <c r="D250" t="s">
@@ -7891,7 +7901,7 @@
         <v>621</v>
       </c>
       <c r="C252">
-        <f>1 * 8760 * 0.297 / (21 * 50000)</f>
+        <f> 1 * 8760 * 0.297 / (21 * 50000)</f>
         <v>0</v>
       </c>
       <c r="D252" t="s">
@@ -7933,7 +7943,7 @@
         <v>621</v>
       </c>
       <c r="C254">
-        <f>1 * 8760 * 0.297 / (21 * 50000)</f>
+        <f> 1 * 8760 * 0.297 / (21 * 50000)</f>
         <v>0</v>
       </c>
       <c r="D254" t="s">
@@ -7975,7 +7985,7 @@
         <v>621</v>
       </c>
       <c r="C256">
-        <f>1 * 8760 * 0.297 / (21 * 50000)</f>
+        <f> 1 * 8760 * 0.297 / (21 * 50000)</f>
         <v>0</v>
       </c>
       <c r="D256" t="s">
@@ -8017,7 +8027,7 @@
         <v>621</v>
       </c>
       <c r="C258">
-        <f>1 * 8760 * 0.297 / (21 * 50000)</f>
+        <f> 1 * 8760 * 0.297 / (21 * 50000)</f>
         <v>0</v>
       </c>
       <c r="D258" t="s">
@@ -8059,7 +8069,7 @@
         <v>621</v>
       </c>
       <c r="C260">
-        <f>1 * 8760 * 0.297 / (21 * 50000)</f>
+        <f> 1 * 8760 * 0.297 / (21 * 50000)</f>
         <v>0</v>
       </c>
       <c r="D260" t="s">
@@ -8101,7 +8111,7 @@
         <v>621</v>
       </c>
       <c r="C262">
-        <f>1 * 8760 * 0.297/ (27 * 32000)</f>
+        <f> 1 * 8760 * 0.297/ (27 * 32000)</f>
         <v>0</v>
       </c>
       <c r="D262" t="s">
@@ -8143,7 +8153,7 @@
         <v>621</v>
       </c>
       <c r="C264">
-        <f>1 * 8760 * 0.297/ (27 * 32000)</f>
+        <f> 1 * 8760 * 0.297/ (27 * 32000)</f>
         <v>0</v>
       </c>
       <c r="D264" t="s">
@@ -8185,7 +8195,7 @@
         <v>621</v>
       </c>
       <c r="C266">
-        <f>1 * 8760 * 0.297/ (27 * 32000)</f>
+        <f> 1 * 8760 * 0.297/ (27 * 32000)</f>
         <v>0</v>
       </c>
       <c r="D266" t="s">
@@ -8227,7 +8237,7 @@
         <v>621</v>
       </c>
       <c r="C268">
-        <f>1 * 8760 * 0.297 / (21 * 50000)</f>
+        <f> 1 * 8760 * 0.297 / (21 * 50000)</f>
         <v>0</v>
       </c>
       <c r="D268" t="s">
@@ -8269,7 +8279,7 @@
         <v>621</v>
       </c>
       <c r="C270">
-        <f>1 * 8760 * 0.297 / (21 * 50000)</f>
+        <f> 1 * 8760 * 0.297 / (21 * 50000)</f>
         <v>0</v>
       </c>
       <c r="D270" t="s">
@@ -8311,7 +8321,7 @@
         <v>621</v>
       </c>
       <c r="C272">
-        <f>1 * 8760 * 0.297 / (21 * 50000)</f>
+        <f> 1 * 8760 * 0.297 / (21 * 50000)</f>
         <v>0</v>
       </c>
       <c r="D272" t="s">
@@ -8517,7 +8527,8 @@
         <v>621</v>
       </c>
       <c r="C282">
-        <f>0.0000000039744 / 6.99719999999999E-10</f>
+        <f> 0.0000000039744 / 0.000000000699719999999999
+</f>
         <v>0</v>
       </c>
       <c r="D282" t="s">
@@ -8552,7 +8563,8 @@
         <v>621</v>
       </c>
       <c r="C284">
-        <f>0.0000000039744 / 6.99719999999999E-10</f>
+        <f> 0.0000000039744 / 0.000000000699719999999999
+</f>
         <v>0</v>
       </c>
       <c r="D284" t="s">
@@ -8629,7 +8641,8 @@
         <v>621</v>
       </c>
       <c r="C288">
-        <f>0.0000000039744 / 6.99719999999999E-10</f>
+        <f> 0.0000000039744 / 0.000000000699719999999999
+</f>
         <v>0</v>
       </c>
       <c r="D288" t="s">
@@ -8664,7 +8677,8 @@
         <v>621</v>
       </c>
       <c r="C290">
-        <f>0.0000000039744 / 6.99719999999999E-10</f>
+        <f> 0.0000000039744 / 0.000000000699719999999999
+</f>
         <v>0</v>
       </c>
       <c r="D290" t="s">
@@ -8824,7 +8838,7 @@
         <v>621</v>
       </c>
       <c r="C299">
-        <f>1 * 8760 * 0.345 / (46 * 150000)</f>
+        <f> 1 * 8760 * 0.345 / (46 * 150000)</f>
         <v>0</v>
       </c>
       <c r="D299" t="s">
@@ -8865,7 +8879,7 @@
         <v>621</v>
       </c>
       <c r="C301">
-        <f>1 * 8760 * 0.345 / (46 * 150000)</f>
+        <f> 1 * 8760 * 0.345 / (46 * 150000)</f>
         <v>0</v>
       </c>
       <c r="D301" t="s">
@@ -8948,7 +8962,7 @@
         <v>621</v>
       </c>
       <c r="C305">
-        <f>3.412969 / (1000 / (8760*0.86)) / 1000000</f>
+        <f> 3.412969 / (1000 / (8760*0.86)) / 1000000</f>
         <v>0</v>
       </c>
       <c r="D305" t="s">
@@ -8969,7 +8983,7 @@
         <v>622</v>
       </c>
       <c r="C306">
-        <f>1 * 3.6 / 43</f>
+        <f> 1 * 3.6 / 43</f>
         <v>0</v>
       </c>
       <c r="D306" t="s">
@@ -9011,7 +9025,7 @@
         <v>622</v>
       </c>
       <c r="C308">
-        <f>3.6 / (41.217 * 0.000001) / 1000000</f>
+        <f> 3.6 / (41.217 * 0.000001) / 1000000</f>
         <v>0</v>
       </c>
       <c r="D308" t="s">
@@ -9184,7 +9198,7 @@
         <v>621</v>
       </c>
       <c r="C317">
-        <f>1 / 2</f>
+        <f> 1 / 2</f>
         <v>0</v>
       </c>
       <c r="D317" t="s">
@@ -9219,7 +9233,7 @@
         <v>621</v>
       </c>
       <c r="C319">
-        <f>1 / 10</f>
+        <f> 1 / 10</f>
         <v>0</v>
       </c>
       <c r="D319" t="s">
@@ -9255,7 +9269,7 @@
         <v>621</v>
       </c>
       <c r="C321">
-        <f>1 / 10</f>
+        <f> 1 / 10</f>
         <v>0</v>
       </c>
       <c r="D321" t="s">
@@ -9308,7 +9322,8 @@
         <v>621</v>
       </c>
       <c r="C324">
-        <f>0.00000044092/0.00000066138</f>
+        <f>0.00000044092/0.00000066138
+</f>
         <v>0</v>
       </c>
       <c r="D324" t="s">
@@ -9329,7 +9344,7 @@
         <v>621</v>
       </c>
       <c r="C325">
-        <f>1 / 50</f>
+        <f> 1 / 50</f>
         <v>0</v>
       </c>
       <c r="D325" t="s">
@@ -9365,7 +9380,7 @@
         <v>621</v>
       </c>
       <c r="C327">
-        <f>0.96 * 1000000 / 50 / 1000000</f>
+        <f> 0.96 * 1000000 / 50 / 1000000</f>
         <v>0</v>
       </c>
       <c r="D327" t="s">
@@ -9458,7 +9473,7 @@
         <v>621</v>
       </c>
       <c r="C332">
-        <f>0.907 * 1000000 / 200 / 1000000</f>
+        <f> 0.907 * 1000000 / 200 / 1000000</f>
         <v>0</v>
       </c>
       <c r="D332" t="s">
@@ -9500,7 +9515,7 @@
         <v>621</v>
       </c>
       <c r="C334">
-        <f>1000/10</f>
+        <f> 1000/10</f>
         <v>0</v>
       </c>
       <c r="D334" t="s">
@@ -9518,7 +9533,8 @@
         <v>621</v>
       </c>
       <c r="C335">
-        <f>0.00000044092/0.00000066138</f>
+        <f>0.00000044092/0.00000066138
+</f>
         <v>0</v>
       </c>
       <c r="D335" t="s">
@@ -9556,7 +9572,7 @@
         <v>621</v>
       </c>
       <c r="C337">
-        <f>0.34 * 1000000 / 200 / 1000000</f>
+        <f> 0.34 * 1000000 / 200 / 1000000</f>
         <v>0</v>
       </c>
       <c r="D337" t="s">
@@ -9671,7 +9687,7 @@
         <v>621</v>
       </c>
       <c r="C343">
-        <f>1 / 10</f>
+        <f> 1 / 10</f>
         <v>0</v>
       </c>
       <c r="D343" t="s">
@@ -9764,7 +9780,8 @@
         <v>621</v>
       </c>
       <c r="C348">
-        <f>0.0000000641/0.000000601</f>
+        <f> 0.0000000641/0.000000601
+</f>
         <v>0</v>
       </c>
       <c r="D348" t="s">
@@ -9838,7 +9855,7 @@
         <v>621</v>
       </c>
       <c r="C352">
-        <f>(1000000 / 100) * 1.0417 / 1000000</f>
+        <f> (1000000 / 100) * 1.0417 / 1000000</f>
         <v>0</v>
       </c>
       <c r="D352" t="s">
@@ -9939,7 +9956,8 @@
         <v>621</v>
       </c>
       <c r="C357">
-        <f>3.89863157894737E-08/0.000000002924</f>
+        <f>0.0000000389863157894737/0.000000002924
+</f>
         <v>0</v>
       </c>
       <c r="D357" t="s">
@@ -9960,7 +9978,7 @@
         <v>621</v>
       </c>
       <c r="C358">
-        <f>1 / 1000</f>
+        <f> 1 / 1000</f>
         <v>0</v>
       </c>
       <c r="D358" t="s">
@@ -10030,7 +10048,7 @@
         <v>621</v>
       </c>
       <c r="C362">
-        <f>1 * 1.25 / 1000</f>
+        <f> 1 * 1.25 / 1000 </f>
         <v>0</v>
       </c>
       <c r="D362" t="s">
@@ -10051,7 +10069,7 @@
         <v>622</v>
       </c>
       <c r="C363">
-        <f>(1000 * 3600) / 0.1636 / 1000000</f>
+        <f> (1000 * 3600) / 0.1636 / 1000000</f>
         <v>0</v>
       </c>
       <c r="D363" t="s">
@@ -10123,7 +10141,7 @@
         <v>621</v>
       </c>
       <c r="C367">
-        <f>1 * 0.44 / 200</f>
+        <f> 1 * 0.44 / 200 </f>
         <v>0</v>
       </c>
       <c r="D367" t="s">
@@ -10165,7 +10183,7 @@
         <v>621</v>
       </c>
       <c r="C369">
-        <f>3.6 * 1000 * 8760 * 0.85 / (100 * 12.35 * 1000000 * 1/2.22)</f>
+        <f> 3.6 * 1000 * 8760 * 0.85 / (100 * 12.35 * 1000000 * 1/2.22)</f>
         <v>0</v>
       </c>
       <c r="D369" t="s">
@@ -10186,7 +10204,7 @@
         <v>621</v>
       </c>
       <c r="C370">
-        <f>1 * 0.44 / 200</f>
+        <f> 1 * 0.44 / 200 </f>
         <v>0</v>
       </c>
       <c r="D370" t="s">
@@ -10228,7 +10246,7 @@
         <v>621</v>
       </c>
       <c r="C372">
-        <f>3.6 * 1000 * 8760 * 0.85 / (100 * 12.35 * 1000000 * 1/2.22)</f>
+        <f> 3.6 * 1000 * 8760 * 0.85 / (100 * 12.35 * 1000000 * 1/2.22)</f>
         <v>0</v>
       </c>
       <c r="D372" t="s">
@@ -10289,7 +10307,7 @@
         <v>621</v>
       </c>
       <c r="C375">
-        <f>(1000000 / 6667)/0.45 / 1000000</f>
+        <f> (1000000 / 6667)/0.45 / 1000000</f>
         <v>0</v>
       </c>
       <c r="D375" t="s">
@@ -10310,7 +10328,7 @@
         <v>622</v>
       </c>
       <c r="C376">
-        <f>(1000 * 3600) / 0.3373 / 1000000</f>
+        <f> (1000 * 3600) / 0.3373 / 1000000</f>
         <v>0</v>
       </c>
       <c r="D376" t="s">
@@ -10385,7 +10403,7 @@
         <v>621</v>
       </c>
       <c r="C380">
-        <f>8760 * 0.85 * 3.6 / 1483 / 1000000</f>
+        <f> 8760 * 0.85 * 3.6 / 1483 / 1000000</f>
         <v>0</v>
       </c>
       <c r="D380" t="s">
@@ -10427,7 +10445,7 @@
         <v>621</v>
       </c>
       <c r="C382">
-        <f>1 / 30</f>
+        <f> 1 / 30</f>
         <v>0</v>
       </c>
       <c r="D382" t="s">
@@ -10502,7 +10520,7 @@
         <v>621</v>
       </c>
       <c r="C386">
-        <f>1 / (16000*846*11.83)</f>
+        <f> 1 / (16000*846*11.83)</f>
         <v>0</v>
       </c>
       <c r="D386" t="s">
@@ -10557,7 +10575,7 @@
         <v>621</v>
       </c>
       <c r="C389">
-        <f>(11.5/0.5) * (1700/500) / 1000000</f>
+        <f> (11.5/0.5) * (1700/500) / 1000000</f>
         <v>0</v>
       </c>
       <c r="D389" t="s">
@@ -10697,7 +10715,7 @@
         <v>622</v>
       </c>
       <c r="C396">
-        <f>3.6 * 1000000 / 50.285 / 1000000</f>
+        <f> 3.6 * 1000000 / 50.285 / 1000000</f>
         <v>0</v>
       </c>
       <c r="D396" t="s">
@@ -10739,7 +10757,7 @@
         <v>622</v>
       </c>
       <c r="C398">
-        <f>3.6 * 1000000 / 14.55 / 1000000</f>
+        <f> 3.6 * 1000000 / 14.55 / 1000000</f>
         <v>0</v>
       </c>
       <c r="D398" t="s">
@@ -10781,7 +10799,7 @@
         <v>622</v>
       </c>
       <c r="C400">
-        <f>3.6 * 1000000 / 50.285 / 1000000</f>
+        <f> 3.6 * 1000000 / 50.285 / 1000000</f>
         <v>0</v>
       </c>
       <c r="D400" t="s">
@@ -10844,7 +10862,7 @@
         <v>622</v>
       </c>
       <c r="C403">
-        <f>3.6 * 1000000 / 43 / 1000000</f>
+        <f> 3.6 * 1000000 / 43 / 1000000</f>
         <v>0</v>
       </c>
       <c r="D403" t="s">
@@ -10948,7 +10966,7 @@
         <v>621</v>
       </c>
       <c r="C408">
-        <f>8760*0.85 / 200 / 1000000</f>
+        <f> 8760*0.85 / 200 / 1000000</f>
         <v>0</v>
       </c>
       <c r="D408" t="s">
@@ -10989,7 +11007,7 @@
         <v>621</v>
       </c>
       <c r="C410">
-        <f>8760*0.85 / 200 / 1000000</f>
+        <f> 8760*0.85 / 200 / 1000000</f>
         <v>0</v>
       </c>
       <c r="D410" t="s">
@@ -11030,7 +11048,7 @@
         <v>621</v>
       </c>
       <c r="C412">
-        <f>8760*0.85 / 200 / 1000000</f>
+        <f> 8760*0.85 / 200 / 1000000</f>
         <v>0</v>
       </c>
       <c r="D412" t="s">
@@ -11172,7 +11190,8 @@
         <v>621</v>
       </c>
       <c r="C419">
-        <f>0.00000000254628/5.3483199147628E-10</f>
+        <f>0.00000000254628/0.00000000053483199147628
+</f>
         <v>0</v>
       </c>
       <c r="D419" t="s">
@@ -11214,7 +11233,7 @@
         <v>622</v>
       </c>
       <c r="C421">
-        <f>1 * 3.6 / 23.9</f>
+        <f> 1 * 3.6 / 23.9</f>
         <v>0</v>
       </c>
       <c r="D421" t="s">
@@ -11252,7 +11271,8 @@
         <v>621</v>
       </c>
       <c r="C423">
-        <f>0.00000000254628/5.3483199147628E-10</f>
+        <f>0.00000000254628/0.00000000053483199147628
+</f>
         <v>0</v>
       </c>
       <c r="D423" t="s">
@@ -11291,7 +11311,7 @@
         <v>621</v>
       </c>
       <c r="C425">
-        <f>1 / (16000*737*12.06)</f>
+        <f> 1 / (16000*737*12.06)</f>
         <v>0</v>
       </c>
       <c r="D425" t="s">
@@ -11389,7 +11409,7 @@
         <v>621</v>
       </c>
       <c r="C430">
-        <f>1/27.7 / 1000</f>
+        <f> 1/27.7 / 1000</f>
         <v>0</v>
       </c>
       <c r="D430" t="s">
@@ -11431,7 +11451,7 @@
         <v>621</v>
       </c>
       <c r="C432">
-        <f>1/27.7 / 1000</f>
+        <f> 1/27.7 / 1000</f>
         <v>0</v>
       </c>
       <c r="D432" t="s">
@@ -11473,7 +11493,7 @@
         <v>621</v>
       </c>
       <c r="C434">
-        <f>1/27.7 / 1000</f>
+        <f> 1/27.7 / 1000</f>
         <v>0</v>
       </c>
       <c r="D434" t="s">
@@ -11557,7 +11577,7 @@
         <v>621</v>
       </c>
       <c r="C438">
-        <f>1 / 160</f>
+        <f> 1 / 160</f>
         <v>0</v>
       </c>
       <c r="D438" t="s">
@@ -11620,7 +11640,7 @@
         <v>621</v>
       </c>
       <c r="C441">
-        <f>1 / 160</f>
+        <f> 1 / 160</f>
         <v>0</v>
       </c>
       <c r="D441" t="s">
@@ -11683,7 +11703,7 @@
         <v>621</v>
       </c>
       <c r="C444">
-        <f>1 / 160</f>
+        <f> 1 / 160</f>
         <v>0</v>
       </c>
       <c r="D444" t="s">
@@ -11983,7 +12003,7 @@
         <v>622</v>
       </c>
       <c r="C459">
-        <f>1 * 3.6 / 23.9</f>
+        <f> 1 * 3.6 / 23.9</f>
         <v>0</v>
       </c>
       <c r="D459" t="s">
@@ -12004,7 +12024,7 @@
         <v>621</v>
       </c>
       <c r="C460">
-        <f>1/200</f>
+        <f> 1/200</f>
         <v>0</v>
       </c>
       <c r="D460" t="s">
@@ -12025,7 +12045,7 @@
         <v>622</v>
       </c>
       <c r="C461">
-        <f>1 * 3.6 / (23.9 * 0.4)</f>
+        <f> 1 * 3.6 / (23.9 * 0.4)</f>
         <v>0</v>
       </c>
       <c r="D461" t="s">
@@ -12046,7 +12066,7 @@
         <v>621</v>
       </c>
       <c r="C462">
-        <f>1/5</f>
+        <f> 1/5</f>
         <v>0</v>
       </c>
       <c r="D462" t="s">
@@ -12126,7 +12146,7 @@
         <v>621</v>
       </c>
       <c r="C466">
-        <f>1 / 1000</f>
+        <f> 1 / 1000</f>
         <v>0</v>
       </c>
       <c r="D466" t="s">
@@ -12204,7 +12224,7 @@
         <v>621</v>
       </c>
       <c r="C470">
-        <f>1 / 1000</f>
+        <f> 1 / 1000</f>
         <v>0</v>
       </c>
       <c r="D470" t="s">
@@ -12257,7 +12277,8 @@
         <v>621</v>
       </c>
       <c r="C473">
-        <f>3.89863157894737E-08/0.000000002924</f>
+        <f>0.0000000389863157894737/0.000000002924
+</f>
         <v>0</v>
       </c>
       <c r="D473" t="s">
@@ -12278,7 +12299,7 @@
         <v>621</v>
       </c>
       <c r="C474">
-        <f>3.6 * 8760 * 0.9 / (100 * 12.35 * 1/1.2195) / 1000000</f>
+        <f> 3.6 * 8760 * 0.9 / (100 * 12.35 * 1/1.2195) / 1000000</f>
         <v>0</v>
       </c>
       <c r="D474" t="s">
@@ -12320,7 +12341,7 @@
         <v>621</v>
       </c>
       <c r="C476">
-        <f>3.6 * 8760 * 0.9 / (100 * 12.35 * 1/1.2195) / 1000000</f>
+        <f> 3.6 * 8760 * 0.9 / (100 * 12.35 * 1/1.2195) / 1000000</f>
         <v>0</v>
       </c>
       <c r="D476" t="s">
@@ -12362,7 +12383,7 @@
         <v>621</v>
       </c>
       <c r="C478">
-        <f>1 / 1000</f>
+        <f> 1 / 1000</f>
         <v>0</v>
       </c>
       <c r="D478" t="s">
@@ -12398,7 +12419,7 @@
         <v>621</v>
       </c>
       <c r="C480">
-        <f>0.956 * (1000000000 / 1000000) / 1000000</f>
+        <f> 0.956 * (1000000000 / 1000000) / 1000000</f>
         <v>0</v>
       </c>
       <c r="D480" t="s">
@@ -12419,7 +12440,7 @@
         <v>622</v>
       </c>
       <c r="C481">
-        <f>(1000 * 3600) / 0.1636 / 1000000</f>
+        <f> (1000 * 3600) / 0.1636 / 1000000</f>
         <v>0</v>
       </c>
       <c r="D481" t="s">
@@ -12491,7 +12512,7 @@
         <v>621</v>
       </c>
       <c r="C485">
-        <f>1000 / 1000000</f>
+        <f> 1000 / 1000000</f>
         <v>0</v>
       </c>
       <c r="D485" t="s">
@@ -12527,7 +12548,7 @@
         <v>621</v>
       </c>
       <c r="C487">
-        <f>1000 / 1000000</f>
+        <f> 1000 / 1000000</f>
         <v>0</v>
       </c>
       <c r="D487" t="s">
@@ -12563,7 +12584,7 @@
         <v>621</v>
       </c>
       <c r="C489">
-        <f>3.6 * 8760 * 0.85 / (100 * 12.35 * 1000 * 1/1.2195)</f>
+        <f> 3.6 * 8760 * 0.85 / (100 * 12.35 * 1000 * 1/1.2195)</f>
         <v>0</v>
       </c>
       <c r="D489" t="s">
@@ -12604,7 +12625,7 @@
         <v>621</v>
       </c>
       <c r="C491">
-        <f>3.6 * 8760 * 0.85 / (100 * 12.35 * 1000 * 1/1.2195)</f>
+        <f> 3.6 * 8760 * 0.85 / (100 * 12.35 * 1000 * 1/1.2195)</f>
         <v>0</v>
       </c>
       <c r="D491" t="s">
@@ -12645,7 +12666,7 @@
         <v>621</v>
       </c>
       <c r="C493">
-        <f>(1000000 / 6667)/0.45 / 1000000</f>
+        <f> (1000000 / 6667)/0.45 / 1000000</f>
         <v>0</v>
       </c>
       <c r="D493" t="s">
@@ -12666,7 +12687,7 @@
         <v>622</v>
       </c>
       <c r="C494">
-        <f>(1000 * 3600) / 0.3373 / 1000000</f>
+        <f> (1000 * 3600) / 0.3373 / 1000000</f>
         <v>0</v>
       </c>
       <c r="D494" t="s">
@@ -12773,7 +12794,7 @@
         <v>621</v>
       </c>
       <c r="C500">
-        <f>1 / 10</f>
+        <f> 1 / 10</f>
         <v>0</v>
       </c>
       <c r="D500" t="s">
@@ -12830,7 +12851,7 @@
         <v>621</v>
       </c>
       <c r="C503">
-        <f>1 * 8760 * 0.093 / (0.75 * 22660)</f>
+        <f> 1 * 8760 * 0.093 / (0.75 * 22660)</f>
         <v>0</v>
       </c>
       <c r="D503" t="s">
@@ -12872,7 +12893,7 @@
         <v>621</v>
       </c>
       <c r="C505">
-        <f>1 * 8760 * 0.093 / (0.75 * 22660)</f>
+        <f> 1 * 8760 * 0.093 / (0.75 * 22660)</f>
         <v>0</v>
       </c>
       <c r="D505" t="s">
@@ -12914,7 +12935,7 @@
         <v>621</v>
       </c>
       <c r="C507">
-        <f>1 * 8760 * 0.093 / (0.75 * 22660)</f>
+        <f> 1 * 8760 * 0.093 / (0.75 * 22660)</f>
         <v>0</v>
       </c>
       <c r="D507" t="s">
@@ -12956,7 +12977,7 @@
         <v>621</v>
       </c>
       <c r="C509">
-        <f>1 * 8760 * 0.093 / (0.75 * 22660)</f>
+        <f> 1 * 8760 * 0.093 / (0.75 * 22660)</f>
         <v>0</v>
       </c>
       <c r="D509" t="s">
@@ -12998,7 +13019,7 @@
         <v>621</v>
       </c>
       <c r="C511">
-        <f>1 * 8760 * 0.093 / (0.75 * 22660)</f>
+        <f> 1 * 8760 * 0.093 / (0.75 * 22660)</f>
         <v>0</v>
       </c>
       <c r="D511" t="s">
@@ -13040,7 +13061,7 @@
         <v>621</v>
       </c>
       <c r="C513">
-        <f>1 * 8760 * 0.093 / (0.75 * 22660)</f>
+        <f> 1 * 8760 * 0.093 / (0.75 * 22660)</f>
         <v>0</v>
       </c>
       <c r="D513" t="s">
@@ -13082,7 +13103,7 @@
         <v>621</v>
       </c>
       <c r="C515">
-        <f>1 * 8760 * 0.093 / (0.75 * 22660)</f>
+        <f> 1 * 8760 * 0.093 / (0.75 * 22660)</f>
         <v>0</v>
       </c>
       <c r="D515" t="s">
@@ -13124,7 +13145,7 @@
         <v>621</v>
       </c>
       <c r="C517">
-        <f>1 * 8760 * 0.093 / (0.75 * 22660)</f>
+        <f> 1 * 8760 * 0.093 / (0.75 * 22660)</f>
         <v>0</v>
       </c>
       <c r="D517" t="s">
@@ -13166,7 +13187,7 @@
         <v>621</v>
       </c>
       <c r="C519">
-        <f>1 * 8760 * 0.093 / (0.75 * 22660)</f>
+        <f> 1 * 8760 * 0.093 / (0.75 * 22660)</f>
         <v>0</v>
       </c>
       <c r="D519" t="s">
@@ -13208,7 +13229,7 @@
         <v>621</v>
       </c>
       <c r="C521">
-        <f>1 * 8760 * 0.093 / (0.75 * 22660)</f>
+        <f> 1 * 8760 * 0.093 / (0.75 * 22660)</f>
         <v>0</v>
       </c>
       <c r="D521" t="s">
@@ -13250,7 +13271,7 @@
         <v>621</v>
       </c>
       <c r="C523">
-        <f>1 * 8760 * 0.093 / (0.75 * 22660)</f>
+        <f> 1 * 8760 * 0.093 / (0.75 * 22660)</f>
         <v>0</v>
       </c>
       <c r="D523" t="s">
@@ -13292,7 +13313,7 @@
         <v>621</v>
       </c>
       <c r="C525">
-        <f>1 * 8760 * 0.093 / (0.75 * 22660)</f>
+        <f> 1 * 8760 * 0.093 / (0.75 * 22660)</f>
         <v>0</v>
       </c>
       <c r="D525" t="s">
@@ -13334,7 +13355,7 @@
         <v>621</v>
       </c>
       <c r="C527">
-        <f>1 * 8760 * 0.093 / (0.75 * 22660)</f>
+        <f> 1 * 8760 * 0.093 / (0.75 * 22660)</f>
         <v>0</v>
       </c>
       <c r="D527" t="s">
@@ -13376,7 +13397,7 @@
         <v>621</v>
       </c>
       <c r="C529">
-        <f>1 * 8760 * 0.093 / (0.75 * 22660)</f>
+        <f> 1 * 8760 * 0.093 / (0.75 * 22660)</f>
         <v>0</v>
       </c>
       <c r="D529" t="s">
@@ -13418,7 +13439,7 @@
         <v>621</v>
       </c>
       <c r="C531">
-        <f>1 * 8760 * 0.093 / (0.75 * 22660)</f>
+        <f> 1 * 8760 * 0.093 / (0.75 * 22660)</f>
         <v>0</v>
       </c>
       <c r="D531" t="s">
@@ -13460,7 +13481,7 @@
         <v>621</v>
       </c>
       <c r="C533">
-        <f>1 * 8760 * 0.093 / (0.75 * 22660)</f>
+        <f> 1 * 8760 * 0.093 / (0.75 * 22660)</f>
         <v>0</v>
       </c>
       <c r="D533" t="s">
@@ -13502,7 +13523,7 @@
         <v>621</v>
       </c>
       <c r="C535">
-        <f>1 * 8760 * 0.093 / (0.75 * 22660)</f>
+        <f> 1 * 8760 * 0.093 / (0.75 * 22660)</f>
         <v>0</v>
       </c>
       <c r="D535" t="s">
@@ -13544,7 +13565,7 @@
         <v>621</v>
       </c>
       <c r="C537">
-        <f>1 * 8760 * 0.093 / (0.75 * 22660)</f>
+        <f> 1 * 8760 * 0.093 / (0.75 * 22660)</f>
         <v>0</v>
       </c>
       <c r="D537" t="s">
@@ -13586,7 +13607,7 @@
         <v>621</v>
       </c>
       <c r="C539">
-        <f>1 * 8760 * 0.093 / (0.75 * 22660)</f>
+        <f> 1 * 8760 * 0.093 / (0.75 * 22660)</f>
         <v>0</v>
       </c>
       <c r="D539" t="s">
@@ -13628,7 +13649,7 @@
         <v>621</v>
       </c>
       <c r="C541">
-        <f>1 * 8760 * 0.093 / (0.75 * 22660)</f>
+        <f> 1 * 8760 * 0.093 / (0.75 * 22660)</f>
         <v>0</v>
       </c>
       <c r="D541" t="s">
@@ -13670,7 +13691,7 @@
         <v>621</v>
       </c>
       <c r="C543">
-        <f>1 * 8760 * 0.093 / (0.75 * 22660)</f>
+        <f> 1 * 8760 * 0.093 / (0.75 * 22660)</f>
         <v>0</v>
       </c>
       <c r="D543" t="s">
@@ -13712,7 +13733,7 @@
         <v>621</v>
       </c>
       <c r="C545">
-        <f>1 * 8760 * 0.093 / (0.75 * 22660)</f>
+        <f> 1 * 8760 * 0.093 / (0.75 * 22660)</f>
         <v>0</v>
       </c>
       <c r="D545" t="s">
@@ -13754,7 +13775,7 @@
         <v>621</v>
       </c>
       <c r="C547">
-        <f>1 * 8760 * 0.093 / (0.75 * 22660)</f>
+        <f> 1 * 8760 * 0.093 / (0.75 * 22660)</f>
         <v>0</v>
       </c>
       <c r="D547" t="s">
@@ -13796,7 +13817,7 @@
         <v>621</v>
       </c>
       <c r="C549">
-        <f>1 * 8760 * 0.093 / (0.75 * 22660)</f>
+        <f> 1 * 8760 * 0.093 / (0.75 * 22660)</f>
         <v>0</v>
       </c>
       <c r="D549" t="s">
@@ -13922,7 +13943,7 @@
         <v>622</v>
       </c>
       <c r="C555">
-        <f>3.6 * 1000000 / 50.285 / 1000000</f>
+        <f> 3.6 * 1000000 / 50.285 / 1000000</f>
         <v>0</v>
       </c>
       <c r="D555" t="s">
@@ -13964,7 +13985,7 @@
         <v>622</v>
       </c>
       <c r="C557">
-        <f>1 / 13.1</f>
+        <f> 1 / 13.1</f>
         <v>0</v>
       </c>
       <c r="D557" t="s">
@@ -14006,7 +14027,7 @@
         <v>622</v>
       </c>
       <c r="C559">
-        <f>1 / 5.54</f>
+        <f> 1 / 5.54</f>
         <v>0</v>
       </c>
       <c r="D559" t="s">
@@ -14069,7 +14090,7 @@
         <v>622</v>
       </c>
       <c r="C562">
-        <f>3.6 * 1000000 / 14.55 / 1000000</f>
+        <f> 3.6 * 1000000 / 14.55 / 1000000</f>
         <v>0</v>
       </c>
       <c r="D562" t="s">
@@ -14111,7 +14132,7 @@
         <v>622</v>
       </c>
       <c r="C564">
-        <f>1 / 5.54</f>
+        <f> 1 / 5.54</f>
         <v>0</v>
       </c>
       <c r="D564" t="s">
@@ -14132,7 +14153,7 @@
         <v>621</v>
       </c>
       <c r="C565">
-        <f>3.6 * 8760 * 0.86 / (0.05 * 1000 * 41.833) / 1000000</f>
+        <f> 3.6 * 8760 * 0.86 / (0.05 * 1000 * 41.833) / 1000000</f>
         <v>0</v>
       </c>
       <c r="D565" t="s">
@@ -14153,7 +14174,7 @@
         <v>622</v>
       </c>
       <c r="C566">
-        <f>3.6 * 1000000 / 41.833 / 1000000</f>
+        <f> 3.6 * 1000000 / 41.833 / 1000000</f>
         <v>0</v>
       </c>
       <c r="D566" t="s">
@@ -14195,7 +14216,7 @@
         <v>622</v>
       </c>
       <c r="C568">
-        <f>3.6 * 1000000 / 50.285 / 1000000</f>
+        <f> 3.6 * 1000000 / 50.285 / 1000000</f>
         <v>0</v>
       </c>
       <c r="D568" t="s">
@@ -14234,7 +14255,7 @@
         <v>621</v>
       </c>
       <c r="C570">
-        <f>(0.06/0.0003) * (30/0.3) / 1000000</f>
+        <f> (0.06/0.0003) * (30/0.3) / 1000000</f>
         <v>0</v>
       </c>
       <c r="D570" t="s">
@@ -14339,7 +14360,7 @@
         <v>621</v>
       </c>
       <c r="C575">
-        <f>1 / 300</f>
+        <f> 1 / 300</f>
         <v>0</v>
       </c>
       <c r="D575" t="s">
@@ -14423,7 +14444,7 @@
         <v>621</v>
       </c>
       <c r="C579">
-        <f>1 / 300</f>
+        <f> 1 / 300</f>
         <v>0</v>
       </c>
       <c r="D579" t="s">
@@ -14507,7 +14528,7 @@
         <v>621</v>
       </c>
       <c r="C583">
-        <f>1 / 160</f>
+        <f> 1 / 160</f>
         <v>0</v>
       </c>
       <c r="D583" t="s">
@@ -14570,7 +14591,7 @@
         <v>621</v>
       </c>
       <c r="C586">
-        <f>1 / 160</f>
+        <f> 1 / 160</f>
         <v>0</v>
       </c>
       <c r="D586" t="s">
@@ -14633,7 +14654,7 @@
         <v>621</v>
       </c>
       <c r="C589">
-        <f>1 / 160</f>
+        <f> 1 / 160</f>
         <v>0</v>
       </c>
       <c r="D589" t="s">
@@ -14881,7 +14902,8 @@
         <v>621</v>
       </c>
       <c r="C601">
-        <f>0.00000000254628/5.3483199147628E-10</f>
+        <f>0.00000000254628/0.00000000053483199147628
+</f>
         <v>0</v>
       </c>
       <c r="D601" t="s">
@@ -14981,7 +15003,7 @@
         <v>622</v>
       </c>
       <c r="C606">
-        <f>3.6 * 2.5</f>
+        <f> 3.6 * 2.5</f>
         <v>0</v>
       </c>
       <c r="D606" t="s">
@@ -15020,7 +15042,7 @@
         <v>622</v>
       </c>
       <c r="C608">
-        <f>3.6 * 2.5</f>
+        <f> 3.6 * 2.5</f>
         <v>0</v>
       </c>
       <c r="D608" t="s">
@@ -15443,7 +15465,7 @@
         <v>621</v>
       </c>
       <c r="C630">
-        <f>1 * 8760 * 0.6 / (57 * 55000000/25)</f>
+        <f> 1 * 8760 * 0.6 / (57 * 55000000/25)</f>
         <v>0</v>
       </c>
       <c r="D630" t="s">
@@ -15485,7 +15507,7 @@
         <v>621</v>
       </c>
       <c r="C632">
-        <f>1 * 8760 * 0.444 / (265 * 49000000/25)</f>
+        <f> 1 * 8760 * 0.444 / (265 * 49000000/25)</f>
         <v>0</v>
       </c>
       <c r="D632" t="s">
@@ -15527,7 +15549,7 @@
         <v>621</v>
       </c>
       <c r="C634">
-        <f>1 * 8760 * 0.349 / (130 * 49000000/25)</f>
+        <f> 1 * 8760 * 0.349 / (130 * 49000000/25)</f>
         <v>0</v>
       </c>
       <c r="D634" t="s">
@@ -15783,7 +15805,7 @@
         <v>621</v>
       </c>
       <c r="C647">
-        <f>8760 * 0.85 / (0.05 * 1000 * 11.28) / 1000000</f>
+        <f> 8760 * 0.85 / (0.05 * 1000 * 11.28) / 1000000</f>
         <v>0</v>
       </c>
       <c r="D647" t="s">
@@ -15825,7 +15847,7 @@
         <v>621</v>
       </c>
       <c r="C649">
-        <f>1 * 8760 * 0.297 / (47 * 24000)</f>
+        <f> 1 * 8760 * 0.297 / (47 * 24000)</f>
         <v>0</v>
       </c>
       <c r="D649" t="s">
@@ -15867,7 +15889,7 @@
         <v>621</v>
       </c>
       <c r="C651">
-        <f>1 * 8760 * 0.297 / (47 * 24000)</f>
+        <f> 1 * 8760 * 0.297 / (47 * 24000)</f>
         <v>0</v>
       </c>
       <c r="D651" t="s">
@@ -15909,7 +15931,7 @@
         <v>621</v>
       </c>
       <c r="C653">
-        <f>1 * 8760 * 0.297 / (47 * 24000)</f>
+        <f> 1 * 8760 * 0.297 / (47 * 24000)</f>
         <v>0</v>
       </c>
       <c r="D653" t="s">
@@ -15951,7 +15973,7 @@
         <v>621</v>
       </c>
       <c r="C655">
-        <f>1 * 8760 * 0.297 / (47 * 24000)</f>
+        <f> 1 * 8760 * 0.297 / (47 * 24000)</f>
         <v>0</v>
       </c>
       <c r="D655" t="s">
@@ -15993,7 +16015,7 @@
         <v>621</v>
       </c>
       <c r="C657">
-        <f>1 * 8760 * 0.297 / (47 * 24000)</f>
+        <f> 1 * 8760 * 0.297 / (47 * 24000)</f>
         <v>0</v>
       </c>
       <c r="D657" t="s">
@@ -16035,7 +16057,7 @@
         <v>621</v>
       </c>
       <c r="C659">
-        <f>1 * 8760 * 0.297 / (47 * 24000)</f>
+        <f> 1 * 8760 * 0.297 / (47 * 24000)</f>
         <v>0</v>
       </c>
       <c r="D659" t="s">
@@ -16077,7 +16099,7 @@
         <v>621</v>
       </c>
       <c r="C661">
-        <f>1 * 8760 * 0.297 / (47 * 24000)</f>
+        <f> 1 * 8760 * 0.297 / (47 * 24000)</f>
         <v>0</v>
       </c>
       <c r="D661" t="s">
@@ -16119,7 +16141,7 @@
         <v>621</v>
       </c>
       <c r="C663">
-        <f>1 * 8760 * 0.297 / (47 * 24000)</f>
+        <f> 1 * 8760 * 0.297 / (47 * 24000)</f>
         <v>0</v>
       </c>
       <c r="D663" t="s">
@@ -16161,7 +16183,7 @@
         <v>621</v>
       </c>
       <c r="C665">
-        <f>1 * 8760 * 0.297 / (47 * 24000)</f>
+        <f> 1 * 8760 * 0.297 / (47 * 24000)</f>
         <v>0</v>
       </c>
       <c r="D665" t="s">
@@ -16203,7 +16225,7 @@
         <v>621</v>
       </c>
       <c r="C667">
-        <f>1 * 8760 * 0.297 / (47 * 24000)</f>
+        <f> 1 * 8760 * 0.297 / (47 * 24000)</f>
         <v>0</v>
       </c>
       <c r="D667" t="s">
@@ -16245,7 +16267,7 @@
         <v>621</v>
       </c>
       <c r="C669">
-        <f>1 * 8760 * 0.093 / (13.4 * 108000)</f>
+        <f> 1 * 8760 * 0.093 / (13.4 * 108000)</f>
         <v>0</v>
       </c>
       <c r="D669" t="s">
@@ -16287,7 +16309,7 @@
         <v>621</v>
       </c>
       <c r="C671">
-        <f>1 * 8760 * 0.093 / (13.4 * 108000)</f>
+        <f> 1 * 8760 * 0.093 / (13.4 * 108000)</f>
         <v>0</v>
       </c>
       <c r="D671" t="s">
@@ -16329,7 +16351,7 @@
         <v>621</v>
       </c>
       <c r="C673">
-        <f>1 * 8760 * 0.093 / (11.7 * 274000)</f>
+        <f> 1 * 8760 * 0.093 / (11.7 * 274000)</f>
         <v>0</v>
       </c>
       <c r="D673" t="s">
@@ -16371,7 +16393,7 @@
         <v>621</v>
       </c>
       <c r="C675">
-        <f>1 * 8760 * 0.093 / (11.7 * 274000)</f>
+        <f> 1 * 8760 * 0.093 / (11.7 * 274000)</f>
         <v>0</v>
       </c>
       <c r="D675" t="s">
@@ -16413,7 +16435,7 @@
         <v>621</v>
       </c>
       <c r="C677">
-        <f>1 * 8760 * 0.093 / (11.7 * 274000)</f>
+        <f> 1 * 8760 * 0.093 / (11.7 * 274000)</f>
         <v>0</v>
       </c>
       <c r="D677" t="s">
@@ -16455,7 +16477,7 @@
         <v>621</v>
       </c>
       <c r="C679">
-        <f>1 * 8760 * 0.093 / (11.7 * 274000)</f>
+        <f> 1 * 8760 * 0.093 / (11.7 * 274000)</f>
         <v>0</v>
       </c>
       <c r="D679" t="s">
@@ -16497,7 +16519,7 @@
         <v>621</v>
       </c>
       <c r="C681">
-        <f>1 * 8760 * 0.093 / (11.7 * 274000)</f>
+        <f> 1 * 8760 * 0.093 / (11.7 * 274000)</f>
         <v>0</v>
       </c>
       <c r="D681" t="s">
@@ -16539,7 +16561,7 @@
         <v>621</v>
       </c>
       <c r="C683">
-        <f>1 * 8760 * 0.093 / (11.7 * 274000)</f>
+        <f> 1 * 8760 * 0.093 / (11.7 * 274000)</f>
         <v>0</v>
       </c>
       <c r="D683" t="s">
@@ -16581,7 +16603,7 @@
         <v>621</v>
       </c>
       <c r="C685">
-        <f>1 * 8760 * 0.093 / (11.7 * 274000)</f>
+        <f> 1 * 8760 * 0.093 / (11.7 * 274000)</f>
         <v>0</v>
       </c>
       <c r="D685" t="s">
@@ -16623,7 +16645,7 @@
         <v>621</v>
       </c>
       <c r="C687">
-        <f>1 * 8760 * 0.093 / (11.7 * 274000)</f>
+        <f> 1 * 8760 * 0.093 / (11.7 * 274000)</f>
         <v>0</v>
       </c>
       <c r="D687" t="s">
@@ -16665,7 +16687,7 @@
         <v>621</v>
       </c>
       <c r="C689">
-        <f>1 * 8760 * 0.093 / (11.7 * 274000)</f>
+        <f> 1 * 8760 * 0.093 / (11.7 * 274000)</f>
         <v>0</v>
       </c>
       <c r="D689" t="s">
@@ -16707,7 +16729,7 @@
         <v>621</v>
       </c>
       <c r="C691">
-        <f>1 * 8760 * 0.093 / (11.7 * 274000)</f>
+        <f> 1 * 8760 * 0.093 / (11.7 * 274000)</f>
         <v>0</v>
       </c>
       <c r="D691" t="s">
@@ -16749,7 +16771,7 @@
         <v>621</v>
       </c>
       <c r="C693">
-        <f>1 * 8760 * 0.093 / (11.7 * 274000)</f>
+        <f> 1 * 8760 * 0.093 / (11.7 * 274000)</f>
         <v>0</v>
       </c>
       <c r="D693" t="s">
@@ -16791,7 +16813,7 @@
         <v>621</v>
       </c>
       <c r="C695">
-        <f>1 * 8760 * 0.093 / (11.7 * 274000)</f>
+        <f> 1 * 8760 * 0.093 / (11.7 * 274000)</f>
         <v>0</v>
       </c>
       <c r="D695" t="s">
@@ -16833,7 +16855,7 @@
         <v>621</v>
       </c>
       <c r="C697">
-        <f>1 * 8760 * 0.093 / (11.7 * 274000)</f>
+        <f> 1 * 8760 * 0.093 / (11.7 * 274000)</f>
         <v>0</v>
       </c>
       <c r="D697" t="s">
@@ -16875,7 +16897,7 @@
         <v>621</v>
       </c>
       <c r="C699">
-        <f>1 * 8760 * 0.093 / (11.7 * 274000)</f>
+        <f> 1 * 8760 * 0.093 / (11.7 * 274000)</f>
         <v>0</v>
       </c>
       <c r="D699" t="s">
@@ -16917,7 +16939,7 @@
         <v>621</v>
       </c>
       <c r="C701">
-        <f>1 * 8760 * 0.093 / (11.7 * 274000)</f>
+        <f> 1 * 8760 * 0.093 / (11.7 * 274000)</f>
         <v>0</v>
       </c>
       <c r="D701" t="s">
@@ -16959,7 +16981,7 @@
         <v>621</v>
       </c>
       <c r="C703">
-        <f>1 * 8760 * 0.093 / (11.7 * 274000)</f>
+        <f> 1 * 8760 * 0.093 / (11.7 * 274000)</f>
         <v>0</v>
       </c>
       <c r="D703" t="s">
@@ -17001,7 +17023,7 @@
         <v>621</v>
       </c>
       <c r="C705">
-        <f>1 * 8760 * 0.093 / (6.3 * 73000)</f>
+        <f> 1 * 8760 * 0.093 / (6.3 * 73000)</f>
         <v>0</v>
       </c>
       <c r="D705" t="s">
@@ -17043,7 +17065,7 @@
         <v>621</v>
       </c>
       <c r="C707">
-        <f>1 * 8760 * 0.093 / (6.3 * 73000)</f>
+        <f> 1 * 8760 * 0.093 / (6.3 * 73000)</f>
         <v>0</v>
       </c>
       <c r="D707" t="s">
@@ -17085,7 +17107,7 @@
         <v>621</v>
       </c>
       <c r="C709">
-        <f>1 * 8760 * 0.093 / (6.3 * 73000)</f>
+        <f> 1 * 8760 * 0.093 / (6.3 * 73000)</f>
         <v>0</v>
       </c>
       <c r="D709" t="s">
@@ -17127,7 +17149,7 @@
         <v>621</v>
       </c>
       <c r="C711">
-        <f>1 * 8760 * 0.093 / (6.3 * 73000)</f>
+        <f> 1 * 8760 * 0.093 / (6.3 * 73000)</f>
         <v>0</v>
       </c>
       <c r="D711" t="s">
@@ -17169,7 +17191,7 @@
         <v>621</v>
       </c>
       <c r="C713">
-        <f>1 * 8760 * 0.093 / (6.3 * 73000)</f>
+        <f> 1 * 8760 * 0.093 / (6.3 * 73000)</f>
         <v>0</v>
       </c>
       <c r="D713" t="s">
@@ -17211,7 +17233,7 @@
         <v>621</v>
       </c>
       <c r="C715">
-        <f>1 * 8760 * 0.093 / (6.3 * 73000)</f>
+        <f> 1 * 8760 * 0.093 / (6.3 * 73000)</f>
         <v>0</v>
       </c>
       <c r="D715" t="s">
@@ -17253,7 +17275,7 @@
         <v>621</v>
       </c>
       <c r="C717">
-        <f>1 * 8760 * 0.093 / (6.3 * 73000)</f>
+        <f> 1 * 8760 * 0.093 / (6.3 * 73000)</f>
         <v>0</v>
       </c>
       <c r="D717" t="s">
@@ -17295,7 +17317,7 @@
         <v>621</v>
       </c>
       <c r="C719">
-        <f>1 * 8760 * 0.093 / (6.3 * 73000)</f>
+        <f> 1 * 8760 * 0.093 / (6.3 * 73000)</f>
         <v>0</v>
       </c>
       <c r="D719" t="s">
@@ -17337,7 +17359,7 @@
         <v>621</v>
       </c>
       <c r="C721">
-        <f>1 * 8760 * 0.093 / (6.3 * 73000)</f>
+        <f> 1 * 8760 * 0.093 / (6.3 * 73000)</f>
         <v>0</v>
       </c>
       <c r="D721" t="s">
@@ -17521,7 +17543,8 @@
         <v>621</v>
       </c>
       <c r="C730">
-        <f>0.00000000254628/5.3483199147628E-10</f>
+        <f>0.00000000254628/0.00000000053483199147628
+</f>
         <v>0</v>
       </c>
       <c r="D730" t="s">
@@ -17559,7 +17582,8 @@
         <v>621</v>
       </c>
       <c r="C732">
-        <f>0.00000000254628/5.3483199147628E-10</f>
+        <f>0.00000000254628/0.00000000053483199147628
+</f>
         <v>0</v>
       </c>
       <c r="D732" t="s">
@@ -17767,7 +17791,7 @@
         <v>621</v>
       </c>
       <c r="C743">
-        <f>(8760*0.85)/130 / 1000000</f>
+        <f> (8760*0.85)/130 / 1000000</f>
         <v>0</v>
       </c>
       <c r="D743" t="s">
@@ -17808,7 +17832,7 @@
         <v>621</v>
       </c>
       <c r="C745">
-        <f>(8760*0.85)/130 / 1000000</f>
+        <f> (8760*0.85)/130 / 1000000</f>
         <v>0</v>
       </c>
       <c r="D745" t="s">
@@ -17849,7 +17873,7 @@
         <v>621</v>
       </c>
       <c r="C747">
-        <f>(8760*0.85)/130 / 1000000</f>
+        <f> (8760*0.85)/130 / 1000000</f>
         <v>0</v>
       </c>
       <c r="D747" t="s">
@@ -17949,7 +17973,7 @@
         <v>621</v>
       </c>
       <c r="C752">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D752" t="s">
@@ -17991,7 +18015,7 @@
         <v>621</v>
       </c>
       <c r="C754">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D754" t="s">
@@ -18033,7 +18057,7 @@
         <v>621</v>
       </c>
       <c r="C756">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D756" t="s">
@@ -18075,7 +18099,7 @@
         <v>621</v>
       </c>
       <c r="C758">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D758" t="s">
@@ -18117,7 +18141,7 @@
         <v>621</v>
       </c>
       <c r="C760">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D760" t="s">
@@ -18159,7 +18183,7 @@
         <v>621</v>
       </c>
       <c r="C762">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D762" t="s">
@@ -18201,7 +18225,7 @@
         <v>621</v>
       </c>
       <c r="C764">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D764" t="s">
@@ -18243,7 +18267,7 @@
         <v>621</v>
       </c>
       <c r="C766">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D766" t="s">
@@ -18285,7 +18309,7 @@
         <v>621</v>
       </c>
       <c r="C768">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D768" t="s">
@@ -18327,7 +18351,7 @@
         <v>621</v>
       </c>
       <c r="C770">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D770" t="s">
@@ -18369,7 +18393,7 @@
         <v>621</v>
       </c>
       <c r="C772">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D772" t="s">
@@ -18411,7 +18435,7 @@
         <v>621</v>
       </c>
       <c r="C774">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D774" t="s">
@@ -18453,7 +18477,7 @@
         <v>621</v>
       </c>
       <c r="C776">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D776" t="s">
@@ -18495,7 +18519,7 @@
         <v>621</v>
       </c>
       <c r="C778">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D778" t="s">
@@ -18537,7 +18561,7 @@
         <v>621</v>
       </c>
       <c r="C780">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D780" t="s">
@@ -18579,7 +18603,7 @@
         <v>621</v>
       </c>
       <c r="C782">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D782" t="s">
@@ -18621,7 +18645,7 @@
         <v>621</v>
       </c>
       <c r="C784">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D784" t="s">
@@ -18663,7 +18687,7 @@
         <v>621</v>
       </c>
       <c r="C786">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D786" t="s">
@@ -18705,7 +18729,7 @@
         <v>621</v>
       </c>
       <c r="C788">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D788" t="s">
@@ -18747,7 +18771,7 @@
         <v>621</v>
       </c>
       <c r="C790">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D790" t="s">
@@ -18789,7 +18813,7 @@
         <v>621</v>
       </c>
       <c r="C792">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D792" t="s">
@@ -18831,7 +18855,7 @@
         <v>621</v>
       </c>
       <c r="C794">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D794" t="s">
@@ -18873,7 +18897,7 @@
         <v>621</v>
       </c>
       <c r="C796">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D796" t="s">
@@ -18915,7 +18939,7 @@
         <v>621</v>
       </c>
       <c r="C798">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D798" t="s">
@@ -18957,7 +18981,7 @@
         <v>621</v>
       </c>
       <c r="C800">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D800" t="s">
@@ -18999,7 +19023,7 @@
         <v>621</v>
       </c>
       <c r="C802">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D802" t="s">
@@ -19041,7 +19065,7 @@
         <v>621</v>
       </c>
       <c r="C804">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D804" t="s">
@@ -19083,7 +19107,7 @@
         <v>621</v>
       </c>
       <c r="C806">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D806" t="s">
@@ -19125,7 +19149,7 @@
         <v>621</v>
       </c>
       <c r="C808">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D808" t="s">
@@ -19167,7 +19191,7 @@
         <v>621</v>
       </c>
       <c r="C810">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D810" t="s">
@@ -19209,7 +19233,7 @@
         <v>621</v>
       </c>
       <c r="C812">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D812" t="s">
@@ -19251,7 +19275,7 @@
         <v>621</v>
       </c>
       <c r="C814">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D814" t="s">
@@ -19293,7 +19317,7 @@
         <v>621</v>
       </c>
       <c r="C816">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D816" t="s">
@@ -19335,7 +19359,7 @@
         <v>621</v>
       </c>
       <c r="C818">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D818" t="s">
@@ -19377,7 +19401,7 @@
         <v>621</v>
       </c>
       <c r="C820">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D820" t="s">
@@ -19419,7 +19443,7 @@
         <v>621</v>
       </c>
       <c r="C822">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D822" t="s">
@@ -19461,7 +19485,7 @@
         <v>621</v>
       </c>
       <c r="C824">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D824" t="s">
@@ -19503,7 +19527,7 @@
         <v>621</v>
       </c>
       <c r="C826">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D826" t="s">
@@ -19545,7 +19569,7 @@
         <v>621</v>
       </c>
       <c r="C828">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D828" t="s">
@@ -19587,7 +19611,7 @@
         <v>621</v>
       </c>
       <c r="C830">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D830" t="s">
@@ -19629,7 +19653,7 @@
         <v>621</v>
       </c>
       <c r="C832">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D832" t="s">
@@ -19671,7 +19695,7 @@
         <v>621</v>
       </c>
       <c r="C834">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D834" t="s">
@@ -19713,7 +19737,7 @@
         <v>621</v>
       </c>
       <c r="C836">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D836" t="s">
@@ -19755,7 +19779,7 @@
         <v>621</v>
       </c>
       <c r="C838">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D838" t="s">
@@ -19797,7 +19821,7 @@
         <v>621</v>
       </c>
       <c r="C840">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D840" t="s">
@@ -19839,7 +19863,7 @@
         <v>621</v>
       </c>
       <c r="C842">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D842" t="s">
@@ -19881,7 +19905,7 @@
         <v>621</v>
       </c>
       <c r="C844">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D844" t="s">
@@ -19923,7 +19947,7 @@
         <v>621</v>
       </c>
       <c r="C846">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D846" t="s">
@@ -19965,7 +19989,7 @@
         <v>621</v>
       </c>
       <c r="C848">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D848" t="s">
@@ -20007,7 +20031,7 @@
         <v>621</v>
       </c>
       <c r="C850">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D850" t="s">
@@ -20049,7 +20073,7 @@
         <v>621</v>
       </c>
       <c r="C852">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D852" t="s">
@@ -20091,7 +20115,7 @@
         <v>621</v>
       </c>
       <c r="C854">
-        <f>1 * 8760 * 0.051 / (1.23 * 12000)</f>
+        <f> 1 * 8760 * 0.051 / (1.23 * 12000)</f>
         <v>0</v>
       </c>
       <c r="D854" t="s">
@@ -20298,7 +20322,7 @@
         <v>621</v>
       </c>
       <c r="C865">
-        <f>1 * 8760 * 0.275 / (343 * (20000000/40))</f>
+        <f> 1 * 8760 * 0.275 / (343 * (20000000/40))</f>
         <v>0</v>
       </c>
       <c r="D865" t="s">
@@ -20340,7 +20364,7 @@
         <v>621</v>
       </c>
       <c r="C867">
-        <f>1 * 8760 * 0.275 / (343 * (20000000/40))</f>
+        <f> 1 * 8760 * 0.275 / (343 * (20000000/40))</f>
         <v>0</v>
       </c>
       <c r="D867" t="s">
@@ -20382,7 +20406,7 @@
         <v>621</v>
       </c>
       <c r="C869">
-        <f>1 * 8760 * 0.275 / (343 * 400000)</f>
+        <f> 1 * 8760 * 0.275 / (343 * 400000)</f>
         <v>0</v>
       </c>
       <c r="D869" t="s">
@@ -20424,7 +20448,7 @@
         <v>621</v>
       </c>
       <c r="C871">
-        <f>1 * 8760 * 0.275 / (343 * 400000)</f>
+        <f> 1 * 8760 * 0.275 / (343 * 400000)</f>
         <v>0</v>
       </c>
       <c r="D871" t="s">
@@ -20466,7 +20490,7 @@
         <v>621</v>
       </c>
       <c r="C873">
-        <f>(1000000 * 40 * 8760 * 0.342) / (9600000 * 20 * 26) / 1000000</f>
+        <f> (1000000 * 40 * 8760 * 0.342) / (9600000 * 20 * 26) / 1000000</f>
         <v>0</v>
       </c>
       <c r="D873" t="s">
@@ -20547,7 +20571,7 @@
         <v>621</v>
       </c>
       <c r="C877">
-        <f>(1000000 * 40 * 8760 * 0.342) / (9600000 * 20 * 26) / 1000000</f>
+        <f> (1000000 * 40 * 8760 * 0.342) / (9600000 * 20 * 26) / 1000000</f>
         <v>0</v>
       </c>
       <c r="D877" t="s">
@@ -20628,7 +20652,7 @@
         <v>621</v>
       </c>
       <c r="C881">
-        <f>(1000000 * 40 * 8760 * 0.342) / (9600000 * 20 * 26) / 1000000</f>
+        <f> (1000000 * 40 * 8760 * 0.342) / (9600000 * 20 * 26) / 1000000</f>
         <v>0</v>
       </c>
       <c r="D881" t="s">
@@ -20709,7 +20733,7 @@
         <v>621</v>
       </c>
       <c r="C885">
-        <f>(1000000 * 40 * 8760 * 0.342) / (9600000 * 20 * 26) / 1000000</f>
+        <f> (1000000 * 40 * 8760 * 0.342) / (9600000 * 20 * 26) / 1000000</f>
         <v>0</v>
       </c>
       <c r="D885" t="s">
@@ -20790,7 +20814,7 @@
         <v>621</v>
       </c>
       <c r="C889">
-        <f>(1000000 * 40 * 8760 * 0.342) / (9600000 * 20 * 26) / 1000000</f>
+        <f> (1000000 * 40 * 8760 * 0.342) / (9600000 * 20 * 26) / 1000000</f>
         <v>0</v>
       </c>
       <c r="D889" t="s">
@@ -20871,7 +20895,7 @@
         <v>621</v>
       </c>
       <c r="C893">
-        <f>(1000000 * 40 * 8760 * 0.342) / (9600000 * 20 * 26) / 1000000</f>
+        <f> (1000000 * 40 * 8760 * 0.342) / (9600000 * 20 * 26) / 1000000</f>
         <v>0</v>
       </c>
       <c r="D893" t="s">
@@ -20953,7 +20977,7 @@
         <v>621</v>
       </c>
       <c r="C897">
-        <f>(1000000 * 40 * 8760 * 0.342) / (9600000 * 20 * 26) / 1000000</f>
+        <f> (1000000 * 40 * 8760 * 0.342) / (9600000 * 20 * 26) / 1000000</f>
         <v>0</v>
       </c>
       <c r="D897" t="s">
@@ -21035,7 +21059,7 @@
         <v>621</v>
       </c>
       <c r="C901">
-        <f>(1000000 * 40 * 8760 * 0.342) / (9600000 * 20 * 26) / 1000000</f>
+        <f> (1000000 * 40 * 8760 * 0.342) / (9600000 * 20 * 26) / 1000000</f>
         <v>0</v>
       </c>
       <c r="D901" t="s">
@@ -21116,7 +21140,7 @@
         <v>621</v>
       </c>
       <c r="C905">
-        <f>(1000000 * 40 * 8760 * 0.342) / (9600000 * 20 * 26) / 1000000</f>
+        <f> (1000000 * 40 * 8760 * 0.342) / (9600000 * 20 * 26) / 1000000</f>
         <v>0</v>
       </c>
       <c r="D905" t="s">
@@ -21197,7 +21221,7 @@
         <v>621</v>
       </c>
       <c r="C909">
-        <f>(1000000 * 40 * 8760 * 0.342) / (9600000 * 20 * 26) / 1000000</f>
+        <f> (1000000 * 40 * 8760 * 0.342) / (9600000 * 20 * 26) / 1000000</f>
         <v>0</v>
       </c>
       <c r="D909" t="s">
@@ -21278,7 +21302,7 @@
         <v>621</v>
       </c>
       <c r="C913">
-        <f>40 * 8760 * 0.275 * 1000000 / (343 * 20000000) / 1000000</f>
+        <f> 40 * 8760 * 0.275 * 1000000 / (343 * 20000000) / 1000000</f>
         <v>0</v>
       </c>
       <c r="D913" t="s">
@@ -21320,7 +21344,7 @@
         <v>621</v>
       </c>
       <c r="C915">
-        <f>40 * 8760 * 0.275 * 1000000 / (343 * 20000000) / 1000000</f>
+        <f> 40 * 8760 * 0.275 * 1000000 / (343 * 20000000) / 1000000</f>
         <v>0</v>
       </c>
       <c r="D915" t="s">
@@ -21362,7 +21386,7 @@
         <v>621</v>
       </c>
       <c r="C917">
-        <f>40 * 8760 * 0.275 * 1000000 / (343 * 20000000) / 1000000</f>
+        <f> 40 * 8760 * 0.275 * 1000000 / (343 * 20000000) / 1000000</f>
         <v>0</v>
       </c>
       <c r="D917" t="s">
@@ -21404,7 +21428,7 @@
         <v>621</v>
       </c>
       <c r="C919">
-        <f>40 * 8760 * 0.275 * 1000000 / (343 * 20000000) / 1000000</f>
+        <f> 40 * 8760 * 0.275 * 1000000 / (343 * 20000000) / 1000000</f>
         <v>0</v>
       </c>
       <c r="D919" t="s">
@@ -21446,7 +21470,7 @@
         <v>621</v>
       </c>
       <c r="C921">
-        <f>1 * 8760 * 0.342 / (28 * 27300)</f>
+        <f> 1 * 8760 * 0.342 / (28 * 27300)</f>
         <v>0</v>
       </c>
       <c r="D921" t="s">
@@ -21488,7 +21512,7 @@
         <v>621</v>
       </c>
       <c r="C923">
-        <f>1 * 8760 * 0.093 / (7.4 * 98000)</f>
+        <f> 1 * 8760 * 0.093 / (7.4 * 98000)</f>
         <v>0</v>
       </c>
       <c r="D923" t="s">
@@ -21530,7 +21554,7 @@
         <v>621</v>
       </c>
       <c r="C925">
-        <f>1 * 8760 * 0.093 / (7.4 * 98000)</f>
+        <f> 1 * 8760 * 0.093 / (7.4 * 98000)</f>
         <v>0</v>
       </c>
       <c r="D925" t="s">
@@ -21572,7 +21596,7 @@
         <v>621</v>
       </c>
       <c r="C927">
-        <f>1 * 8760 * 0.093 / (7.4 * 98000)</f>
+        <f> 1 * 8760 * 0.093 / (7.4 * 98000)</f>
         <v>0</v>
       </c>
       <c r="D927" t="s">
@@ -21614,7 +21638,7 @@
         <v>621</v>
       </c>
       <c r="C929">
-        <f>1 * 8760 * 0.093 / (7.4 * 98000)</f>
+        <f> 1 * 8760 * 0.093 / (7.4 * 98000)</f>
         <v>0</v>
       </c>
       <c r="D929" t="s">
@@ -21656,7 +21680,7 @@
         <v>621</v>
       </c>
       <c r="C931">
-        <f>1 * 8760 * 0.093 / (7.4 * 98000)</f>
+        <f> 1 * 8760 * 0.093 / (7.4 * 98000)</f>
         <v>0</v>
       </c>
       <c r="D931" t="s">
@@ -21698,7 +21722,7 @@
         <v>621</v>
       </c>
       <c r="C933">
-        <f>1 * 8760 * 0.093 / (7.4 * 98000)</f>
+        <f> 1 * 8760 * 0.093 / (7.4 * 98000)</f>
         <v>0</v>
       </c>
       <c r="D933" t="s">
@@ -21740,7 +21764,7 @@
         <v>621</v>
       </c>
       <c r="C935">
-        <f>1 * 8760 * 0.093 / (7.4 * 98000)</f>
+        <f> 1 * 8760 * 0.093 / (7.4 * 98000)</f>
         <v>0</v>
       </c>
       <c r="D935" t="s">
@@ -21782,7 +21806,7 @@
         <v>621</v>
       </c>
       <c r="C937">
-        <f>1 * 8760 * 0.093 / (7.4 * 98000)</f>
+        <f> 1 * 8760 * 0.093 / (7.4 * 98000)</f>
         <v>0</v>
       </c>
       <c r="D937" t="s">
@@ -21824,7 +21848,7 @@
         <v>621</v>
       </c>
       <c r="C939">
-        <f>1 * 8760 * 0.093 / (7.4 * 98000)</f>
+        <f> 1 * 8760 * 0.093 / (7.4 * 98000)</f>
         <v>0</v>
       </c>
       <c r="D939" t="s">
@@ -21866,7 +21890,7 @@
         <v>621</v>
       </c>
       <c r="C941">
-        <f>1 * 8760 * 0.093 / (3.2 * 78000)</f>
+        <f> 1 * 8760 * 0.093 / (3.2 * 78000)</f>
         <v>0</v>
       </c>
       <c r="D941" t="s">
@@ -21908,7 +21932,7 @@
         <v>621</v>
       </c>
       <c r="C943">
-        <f>1 * 8760 * 0.093 / (3.2 * 78000)</f>
+        <f> 1 * 8760 * 0.093 / (3.2 * 78000)</f>
         <v>0</v>
       </c>
       <c r="D943" t="s">
@@ -21950,7 +21974,7 @@
         <v>621</v>
       </c>
       <c r="C945">
-        <f>1 * 8760 * 0.093 / (3.2 * 78000)</f>
+        <f> 1 * 8760 * 0.093 / (3.2 * 78000)</f>
         <v>0</v>
       </c>
       <c r="D945" t="s">
@@ -21992,7 +22016,7 @@
         <v>621</v>
       </c>
       <c r="C947">
-        <f>1 * 8760 * 0.093 / (3.2 * 78000)</f>
+        <f> 1 * 8760 * 0.093 / (3.2 * 78000)</f>
         <v>0</v>
       </c>
       <c r="D947" t="s">
@@ -22034,7 +22058,7 @@
         <v>621</v>
       </c>
       <c r="C949">
-        <f>1 * 8760 * 0.093 / (3.2 * 78000)</f>
+        <f> 1 * 8760 * 0.093 / (3.2 * 78000)</f>
         <v>0</v>
       </c>
       <c r="D949" t="s">
@@ -22076,7 +22100,7 @@
         <v>621</v>
       </c>
       <c r="C951">
-        <f>1 * 8760 * 0.093 / (3.2 * 78000)</f>
+        <f> 1 * 8760 * 0.093 / (3.2 * 78000)</f>
         <v>0</v>
       </c>
       <c r="D951" t="s">
@@ -22118,7 +22142,7 @@
         <v>621</v>
       </c>
       <c r="C953">
-        <f>1 * 8760 * 0.093 / (3.2 * 78000)</f>
+        <f> 1 * 8760 * 0.093 / (3.2 * 78000)</f>
         <v>0</v>
       </c>
       <c r="D953" t="s">
@@ -22160,7 +22184,7 @@
         <v>621</v>
       </c>
       <c r="C955">
-        <f>1 * 8760 * 0.093 / (3.2 * 78000)</f>
+        <f> 1 * 8760 * 0.093 / (3.2 * 78000)</f>
         <v>0</v>
       </c>
       <c r="D955" t="s">
@@ -22202,7 +22226,7 @@
         <v>621</v>
       </c>
       <c r="C957">
-        <f>1 * 8760 * 0.093 / (3.2 * 78000)</f>
+        <f> 1 * 8760 * 0.093 / (3.2 * 78000)</f>
         <v>0</v>
       </c>
       <c r="D957" t="s">
@@ -22244,7 +22268,7 @@
         <v>621</v>
       </c>
       <c r="C959">
-        <f>1 * 8760 * 0.093 / (3.2 * 78000)</f>
+        <f> 1 * 8760 * 0.093 / (3.2 * 78000)</f>
         <v>0</v>
       </c>
       <c r="D959" t="s">
@@ -22286,7 +22310,7 @@
         <v>621</v>
       </c>
       <c r="C961">
-        <f>1 * 8760 * 0.093 / (3.2 * 78000)</f>
+        <f> 1 * 8760 * 0.093 / (3.2 * 78000)</f>
         <v>0</v>
       </c>
       <c r="D961" t="s">
@@ -22328,7 +22352,7 @@
         <v>621</v>
       </c>
       <c r="C963">
-        <f>1 * 8760 * 0.093 / (3.2 * 78000)</f>
+        <f> 1 * 8760 * 0.093 / (3.2 * 78000)</f>
         <v>0</v>
       </c>
       <c r="D963" t="s">
@@ -22370,7 +22394,7 @@
         <v>621</v>
       </c>
       <c r="C965">
-        <f>1 * 8760 * 0.093 / (3.2 * 78000)</f>
+        <f> 1 * 8760 * 0.093 / (3.2 * 78000)</f>
         <v>0</v>
       </c>
       <c r="D965" t="s">
@@ -22412,7 +22436,7 @@
         <v>621</v>
       </c>
       <c r="C967">
-        <f>1 * 8760 * 0.093 / (3.2 * 78000)</f>
+        <f> 1 * 8760 * 0.093 / (3.2 * 78000)</f>
         <v>0</v>
       </c>
       <c r="D967" t="s">
@@ -22454,7 +22478,7 @@
         <v>621</v>
       </c>
       <c r="C969">
-        <f>1 * 8760 * 0.093 / (3.2 * 78000)</f>
+        <f> 1 * 8760 * 0.093 / (3.2 * 78000)</f>
         <v>0</v>
       </c>
       <c r="D969" t="s">
@@ -22496,7 +22520,7 @@
         <v>621</v>
       </c>
       <c r="C971">
-        <f>1 * 8760 * 0.093 / (3.2 * 78000)</f>
+        <f> 1 * 8760 * 0.093 / (3.2 * 78000)</f>
         <v>0</v>
       </c>
       <c r="D971" t="s">
@@ -22538,7 +22562,7 @@
         <v>621</v>
       </c>
       <c r="C973">
-        <f>1 * 8760 * 0.093 / (3.2 * 78000)</f>
+        <f> 1 * 8760 * 0.093 / (3.2 * 78000)</f>
         <v>0</v>
       </c>
       <c r="D973" t="s">
@@ -22580,7 +22604,7 @@
         <v>621</v>
       </c>
       <c r="C975">
-        <f>1 * 8760 * 0.093 / (3.2 * 78000)</f>
+        <f> 1 * 8760 * 0.093 / (3.2 * 78000)</f>
         <v>0</v>
       </c>
       <c r="D975" t="s">
@@ -22927,7 +22951,7 @@
         <v>622</v>
       </c>
       <c r="C993">
-        <f>1 / 5.54</f>
+        <f> 1 / 5.54</f>
         <v>0</v>
       </c>
       <c r="D993" t="s">
@@ -23209,7 +23233,7 @@
         <v>623</v>
       </c>
       <c r="C1007">
-        <f>1/11.28</f>
+        <f> 1/11.28</f>
         <v>0</v>
       </c>
       <c r="D1007" t="s">
@@ -23377,7 +23401,7 @@
         <v>623</v>
       </c>
       <c r="C1015">
-        <f>1 / 12.06</f>
+        <f> 1 / 12.06</f>
         <v>0</v>
       </c>
       <c r="D1015" t="s">

</xml_diff>